<commit_message>
Annot 30 -> 50
</commit_message>
<xml_diff>
--- a/sbs/openai_davinci_003_gusev_13b_ru_alpaca_lora.xlsx
+++ b/sbs/openai_davinci_003_gusev_13b_ru_alpaca_lora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexkuk/proj/rulm-sbs/sbs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DC5481-A1BC-8A46-8AC8-EF920D9B99F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58C129D-2E6C-5F4D-9767-D2459B8CF6D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1610,8 +1610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2195,6 +2195,9 @@
       <c r="D34" s="2" t="s">
         <v>136</v>
       </c>
+      <c r="E34" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="35" spans="1:5" ht="128" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
@@ -2209,6 +2212,9 @@
       <c r="D35" s="2" t="s">
         <v>140</v>
       </c>
+      <c r="E35" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:5" ht="240" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
@@ -2223,6 +2229,9 @@
       <c r="D36" s="2" t="s">
         <v>144</v>
       </c>
+      <c r="E36" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="37" spans="1:5" ht="240" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
@@ -2237,6 +2246,9 @@
       <c r="D37" s="2" t="s">
         <v>148</v>
       </c>
+      <c r="E37" s="2">
+        <v>-2</v>
+      </c>
     </row>
     <row r="38" spans="1:5" ht="160" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
@@ -2251,6 +2263,9 @@
       <c r="D38" s="2" t="s">
         <v>152</v>
       </c>
+      <c r="E38" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:5" ht="208" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
@@ -2265,6 +2280,9 @@
       <c r="D39" s="2" t="s">
         <v>156</v>
       </c>
+      <c r="E39" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:5" ht="112" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
@@ -2279,6 +2297,9 @@
       <c r="D40" s="2" t="s">
         <v>160</v>
       </c>
+      <c r="E40" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="41" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
@@ -2293,6 +2314,9 @@
       <c r="D41" s="2" t="s">
         <v>164</v>
       </c>
+      <c r="E41" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="1:5" ht="192" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
@@ -2307,6 +2331,9 @@
       <c r="D42" s="2" t="s">
         <v>168</v>
       </c>
+      <c r="E42" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="43" spans="1:5" ht="350" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
@@ -2321,6 +2348,9 @@
       <c r="D43" s="2" t="s">
         <v>172</v>
       </c>
+      <c r="E43" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:5" ht="208" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
@@ -2335,6 +2365,9 @@
       <c r="D44" s="2" t="s">
         <v>176</v>
       </c>
+      <c r="E44" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="1:5" ht="224" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
@@ -2349,6 +2382,9 @@
       <c r="D45" s="2" t="s">
         <v>180</v>
       </c>
+      <c r="E45" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="1:5" ht="128" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
@@ -2363,6 +2399,9 @@
       <c r="D46" s="2" t="s">
         <v>184</v>
       </c>
+      <c r="E46" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:5" ht="256" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
@@ -2377,6 +2416,9 @@
       <c r="D47" s="2" t="s">
         <v>188</v>
       </c>
+      <c r="E47" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:5" ht="240" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
@@ -2391,8 +2433,11 @@
       <c r="D48" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" ht="224" x14ac:dyDescent="0.2">
+      <c r="E48" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="224" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>193</v>
       </c>
@@ -2405,8 +2450,11 @@
       <c r="D49" s="2" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+      <c r="E49" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="112" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>197</v>
       </c>
@@ -2419,8 +2467,11 @@
       <c r="D50" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" ht="176" x14ac:dyDescent="0.2">
+      <c r="E50" s="2">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="176" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>201</v>
       </c>
@@ -2433,8 +2484,11 @@
       <c r="D51" s="2" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="E51" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>205</v>
       </c>
@@ -2447,8 +2501,11 @@
       <c r="D52" s="2" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" ht="224" x14ac:dyDescent="0.2">
+      <c r="E52" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="224" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>209</v>
       </c>
@@ -2461,8 +2518,11 @@
       <c r="D53" s="2" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" ht="288" x14ac:dyDescent="0.2">
+      <c r="E53" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="288" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>213</v>
       </c>
@@ -2475,8 +2535,11 @@
       <c r="D54" s="2" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" ht="144" x14ac:dyDescent="0.2">
+      <c r="E54" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="144" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>217</v>
       </c>

</xml_diff>